<commit_message>
Remove Skills Advanced System migration files, including creation and deletion scripts for actions, buffs, and related configurations.
</commit_message>
<xml_diff>
--- a/configs/game/游戏配置表_v1.0.0.0.xlsx
+++ b/configs/game/游戏配置表_v1.0.0.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowHeight="15380" tabRatio="817" activeTab="13"/>
+    <workbookView windowWidth="29100" windowHeight="14620" tabRatio="817"/>
   </bookViews>
   <sheets>
     <sheet name="角色数据类型" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="562">
   <si>
     <t>代码</t>
   </si>
@@ -75,7 +75,7 @@
     <t>力量</t>
   </si>
   <si>
-    <t>Attribute</t>
+    <t>basic</t>
   </si>
   <si>
     <t>integer</t>
@@ -129,7 +129,7 @@
     <t>精准</t>
   </si>
   <si>
-    <t>Data</t>
+    <t>derived</t>
   </si>
   <si>
     <t>命中率计算基础值</t>
@@ -150,7 +150,7 @@
     <t>物理抗性</t>
   </si>
   <si>
-    <t>Resistance</t>
+    <t>resistance</t>
   </si>
   <si>
     <t>percentage</t>
@@ -712,9 +712,6 @@
   </si>
   <si>
     <t>Movement</t>
-  </si>
-  <si>
-    <t>basic</t>
   </si>
   <si>
     <t>[{"action":"movement","unlock_level":1}]</t>
@@ -2737,8 +2734,8 @@
   <sheetPr/>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J$1:J$1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="17.6"/>
@@ -3074,7 +3071,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="A1:I11" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:I1 A2:B11 D2:I11" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -3098,13 +3095,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>428</v>
+      </c>
+      <c r="B1" t="s">
         <v>429</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>430</v>
-      </c>
-      <c r="C1" t="s">
-        <v>431</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
@@ -3115,16 +3112,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B2" t="s">
+        <v>431</v>
+      </c>
+      <c r="C2" t="s">
         <v>432</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>433</v>
-      </c>
-      <c r="D2" t="s">
-        <v>434</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
@@ -3132,16 +3129,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>434</v>
+      </c>
+      <c r="B3" t="s">
         <v>435</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>432</v>
+      </c>
+      <c r="D3" t="s">
         <v>436</v>
-      </c>
-      <c r="C3" t="s">
-        <v>433</v>
-      </c>
-      <c r="D3" t="s">
-        <v>437</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -3152,13 +3149,13 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
+        <v>437</v>
+      </c>
+      <c r="C4" t="s">
         <v>438</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>439</v>
-      </c>
-      <c r="D4" t="s">
-        <v>440</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -3166,16 +3163,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>440</v>
+      </c>
+      <c r="B5" t="s">
         <v>441</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>432</v>
+      </c>
+      <c r="D5" t="s">
         <v>442</v>
-      </c>
-      <c r="C5" t="s">
-        <v>433</v>
-      </c>
-      <c r="D5" t="s">
-        <v>443</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -3183,16 +3180,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
+        <v>443</v>
+      </c>
+      <c r="B6" t="s">
         <v>444</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>445</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>446</v>
-      </c>
-      <c r="D6" t="s">
-        <v>447</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -3200,16 +3197,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
+        <v>447</v>
+      </c>
+      <c r="B7" t="s">
         <v>448</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>438</v>
+      </c>
+      <c r="D7" t="s">
         <v>449</v>
-      </c>
-      <c r="C7" t="s">
-        <v>439</v>
-      </c>
-      <c r="D7" t="s">
-        <v>450</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -3217,16 +3214,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
+        <v>450</v>
+      </c>
+      <c r="B8" t="s">
         <v>451</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>438</v>
+      </c>
+      <c r="D8" t="s">
         <v>452</v>
-      </c>
-      <c r="C8" t="s">
-        <v>439</v>
-      </c>
-      <c r="D8" t="s">
-        <v>453</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -3234,16 +3231,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>224</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
+        <v>453</v>
+      </c>
+      <c r="C9" t="s">
+        <v>438</v>
+      </c>
+      <c r="D9" t="s">
         <v>454</v>
-      </c>
-      <c r="C9" t="s">
-        <v>439</v>
-      </c>
-      <c r="D9" t="s">
-        <v>455</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -3251,16 +3248,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B10" t="s">
+        <v>455</v>
+      </c>
+      <c r="C10" t="s">
+        <v>438</v>
+      </c>
+      <c r="D10" t="s">
         <v>456</v>
-      </c>
-      <c r="C10" t="s">
-        <v>439</v>
-      </c>
-      <c r="D10" t="s">
-        <v>457</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -3268,16 +3265,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
+        <v>457</v>
+      </c>
+      <c r="B11" t="s">
         <v>458</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>445</v>
+      </c>
+      <c r="D11" t="s">
         <v>459</v>
-      </c>
-      <c r="C11" t="s">
-        <v>446</v>
-      </c>
-      <c r="D11" t="s">
-        <v>460</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
@@ -3285,16 +3282,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
+        <v>460</v>
+      </c>
+      <c r="B12" t="s">
         <v>461</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>445</v>
+      </c>
+      <c r="D12" t="s">
         <v>462</v>
-      </c>
-      <c r="C12" t="s">
-        <v>446</v>
-      </c>
-      <c r="D12" t="s">
-        <v>463</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
@@ -3302,16 +3299,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
+        <v>463</v>
+      </c>
+      <c r="B13" t="s">
         <v>464</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>465</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>466</v>
-      </c>
-      <c r="D13" t="s">
-        <v>467</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
@@ -3319,16 +3316,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B14" t="s">
         <v>166</v>
       </c>
       <c r="C14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D14" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E14" t="s">
         <v>14</v>
@@ -3336,16 +3333,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B15" t="s">
         <v>195</v>
       </c>
       <c r="C15" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D15" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E15" t="s">
         <v>14</v>
@@ -3353,16 +3350,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B16" t="s">
         <v>198</v>
       </c>
       <c r="C16" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D16" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E16" t="s">
         <v>14</v>
@@ -3370,16 +3367,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B17" t="s">
         <v>201</v>
       </c>
       <c r="C17" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D17" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E17" t="s">
         <v>14</v>
@@ -3387,16 +3384,16 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
+        <v>472</v>
+      </c>
+      <c r="B18" t="s">
         <v>473</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>474</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>475</v>
-      </c>
-      <c r="D18" t="s">
-        <v>476</v>
       </c>
       <c r="E18" t="s">
         <v>14</v>
@@ -3404,16 +3401,16 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
+        <v>476</v>
+      </c>
+      <c r="B19" t="s">
         <v>477</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>474</v>
+      </c>
+      <c r="D19" t="s">
         <v>478</v>
-      </c>
-      <c r="C19" t="s">
-        <v>475</v>
-      </c>
-      <c r="D19" t="s">
-        <v>479</v>
       </c>
       <c r="E19" t="s">
         <v>14</v>
@@ -3421,16 +3418,16 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
+        <v>479</v>
+      </c>
+      <c r="B20" t="s">
         <v>480</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>474</v>
+      </c>
+      <c r="D20" t="s">
         <v>481</v>
-      </c>
-      <c r="C20" t="s">
-        <v>475</v>
-      </c>
-      <c r="D20" t="s">
-        <v>482</v>
       </c>
       <c r="E20" t="s">
         <v>14</v>
@@ -3464,10 +3461,10 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B1" t="s">
         <v>483</v>
-      </c>
-      <c r="B1" t="s">
-        <v>484</v>
       </c>
       <c r="C1" t="s">
         <v>89</v>
@@ -3476,194 +3473,194 @@
         <v>90</v>
       </c>
       <c r="E1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>485</v>
+      </c>
+      <c r="B2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C2" t="s">
         <v>486</v>
       </c>
-      <c r="B2" t="s">
-        <v>350</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>487</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>488</v>
-      </c>
-      <c r="E2" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B3" t="s">
+        <v>489</v>
+      </c>
+      <c r="C3" t="s">
         <v>490</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>491</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>492</v>
-      </c>
-      <c r="E3" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B4" t="s">
+        <v>493</v>
+      </c>
+      <c r="C4" t="s">
         <v>494</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>495</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>496</v>
-      </c>
-      <c r="E4" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B5" t="s">
+        <v>497</v>
+      </c>
+      <c r="C5" t="s">
         <v>498</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>499</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>500</v>
-      </c>
-      <c r="E5" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B6" t="s">
+        <v>501</v>
+      </c>
+      <c r="C6" t="s">
         <v>502</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>503</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>504</v>
-      </c>
-      <c r="E6" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
+        <v>505</v>
+      </c>
+      <c r="B7" t="s">
         <v>506</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>507</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>508</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>509</v>
-      </c>
-      <c r="E7" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B8" t="s">
+        <v>510</v>
+      </c>
+      <c r="C8" t="s">
         <v>511</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>512</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>513</v>
-      </c>
-      <c r="E8" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B9" t="s">
+        <v>514</v>
+      </c>
+      <c r="C9" t="s">
         <v>515</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>516</v>
       </c>
-      <c r="D9" t="s">
-        <v>517</v>
-      </c>
       <c r="E9" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B10" t="s">
+        <v>517</v>
+      </c>
+      <c r="C10" t="s">
         <v>518</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>519</v>
       </c>
-      <c r="D10" t="s">
-        <v>520</v>
-      </c>
       <c r="E10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
+        <v>520</v>
+      </c>
+      <c r="B11" t="s">
         <v>521</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>522</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>523</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>524</v>
-      </c>
-      <c r="E11" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B12" t="s">
+        <v>525</v>
+      </c>
+      <c r="C12" t="s">
         <v>526</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>527</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>528</v>
-      </c>
-      <c r="E12" t="s">
-        <v>529</v>
       </c>
     </row>
   </sheetData>
@@ -3692,16 +3689,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B1" t="s">
         <v>89</v>
       </c>
       <c r="C1" t="s">
+        <v>529</v>
+      </c>
+      <c r="D1" t="s">
         <v>530</v>
-      </c>
-      <c r="D1" t="s">
-        <v>531</v>
       </c>
       <c r="E1" t="s">
         <v>90</v>
@@ -3709,70 +3706,70 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B2" t="s">
+        <v>531</v>
+      </c>
+      <c r="C2" t="s">
         <v>532</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>533</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>534</v>
-      </c>
-      <c r="E2" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B3" t="s">
+        <v>535</v>
+      </c>
+      <c r="C3" t="s">
+        <v>532</v>
+      </c>
+      <c r="D3" t="s">
+        <v>533</v>
+      </c>
+      <c r="E3" t="s">
         <v>536</v>
-      </c>
-      <c r="C3" t="s">
-        <v>533</v>
-      </c>
-      <c r="D3" t="s">
-        <v>534</v>
-      </c>
-      <c r="E3" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B4" t="s">
+        <v>537</v>
+      </c>
+      <c r="C4" t="s">
+        <v>532</v>
+      </c>
+      <c r="D4" t="s">
         <v>538</v>
       </c>
-      <c r="C4" t="s">
-        <v>533</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>539</v>
-      </c>
-      <c r="E4" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>540</v>
+      </c>
+      <c r="B5" t="s">
         <v>541</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>542</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>543</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>544</v>
-      </c>
-      <c r="E5" t="s">
-        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -3800,13 +3797,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>545</v>
+      </c>
+      <c r="B1" t="s">
         <v>546</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>547</v>
-      </c>
-      <c r="C1" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3933,7 +3930,7 @@
   <sheetPr/>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -3946,10 +3943,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B1" t="s">
         <v>549</v>
-      </c>
-      <c r="B1" t="s">
-        <v>550</v>
       </c>
       <c r="C1" t="s">
         <v>89</v>
@@ -3957,46 +3954,46 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>550</v>
+      </c>
+      <c r="B2" t="s">
         <v>551</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>552</v>
-      </c>
-      <c r="C2" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>553</v>
+      </c>
+      <c r="B3" t="s">
         <v>554</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>555</v>
-      </c>
-      <c r="C3" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B4" t="s">
         <v>557</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>558</v>
-      </c>
-      <c r="C4" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>559</v>
+      </c>
+      <c r="B5" t="s">
         <v>560</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>561</v>
-      </c>
-      <c r="C5" t="s">
-        <v>562</v>
       </c>
     </row>
   </sheetData>
@@ -5110,16 +5107,16 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>224</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
         <v>51</v>
       </c>
       <c r="G4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H4" t="s">
         <v>225</v>
-      </c>
-      <c r="H4" t="s">
-        <v>226</v>
       </c>
       <c r="I4" t="s">
         <v>14</v>
@@ -5127,28 +5124,28 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B5" t="s">
         <v>227</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>228</v>
-      </c>
-      <c r="C5" t="s">
-        <v>229</v>
       </c>
       <c r="D5">
         <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F5" t="s">
         <v>51</v>
       </c>
       <c r="G5" t="s">
+        <v>230</v>
+      </c>
+      <c r="H5" t="s">
         <v>231</v>
-      </c>
-      <c r="H5" t="s">
-        <v>232</v>
       </c>
       <c r="I5" t="s">
         <v>14</v>
@@ -5156,28 +5153,28 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B6" t="s">
         <v>233</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>234</v>
-      </c>
-      <c r="C6" t="s">
-        <v>235</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>224</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
         <v>51</v>
       </c>
       <c r="G6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H6" t="s">
         <v>236</v>
-      </c>
-      <c r="H6" t="s">
-        <v>237</v>
       </c>
       <c r="I6" t="s">
         <v>14</v>
@@ -5185,10 +5182,10 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
+        <v>237</v>
+      </c>
+      <c r="B7" t="s">
         <v>238</v>
-      </c>
-      <c r="B7" t="s">
-        <v>239</v>
       </c>
       <c r="C7" t="s">
         <v>219</v>
@@ -5197,16 +5194,16 @@
         <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F7" t="s">
         <v>51</v>
       </c>
       <c r="G7" t="s">
+        <v>240</v>
+      </c>
+      <c r="H7" t="s">
         <v>241</v>
-      </c>
-      <c r="H7" t="s">
-        <v>242</v>
       </c>
       <c r="I7" t="s">
         <v>14</v>
@@ -5214,28 +5211,28 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
+        <v>242</v>
+      </c>
+      <c r="B8" t="s">
         <v>243</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>244</v>
-      </c>
-      <c r="C8" t="s">
-        <v>245</v>
       </c>
       <c r="D8">
         <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F8" t="s">
         <v>51</v>
       </c>
       <c r="G8" t="s">
+        <v>246</v>
+      </c>
+      <c r="H8" t="s">
         <v>247</v>
-      </c>
-      <c r="H8" t="s">
-        <v>248</v>
       </c>
       <c r="I8" t="s">
         <v>14</v>
@@ -5243,28 +5240,28 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
+        <v>248</v>
+      </c>
+      <c r="B9" t="s">
         <v>249</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>250</v>
-      </c>
-      <c r="C9" t="s">
-        <v>251</v>
       </c>
       <c r="D9">
         <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F9" t="s">
         <v>51</v>
       </c>
       <c r="G9" t="s">
+        <v>252</v>
+      </c>
+      <c r="H9" t="s">
         <v>253</v>
-      </c>
-      <c r="H9" t="s">
-        <v>254</v>
       </c>
       <c r="I9" t="s">
         <v>14</v>
@@ -5272,10 +5269,10 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
+        <v>254</v>
+      </c>
+      <c r="B10" t="s">
         <v>255</v>
-      </c>
-      <c r="B10" t="s">
-        <v>256</v>
       </c>
       <c r="C10" t="s">
         <v>219</v>
@@ -5284,16 +5281,16 @@
         <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F10" t="s">
         <v>51</v>
       </c>
       <c r="G10" t="s">
+        <v>257</v>
+      </c>
+      <c r="H10" t="s">
         <v>258</v>
-      </c>
-      <c r="H10" t="s">
-        <v>259</v>
       </c>
       <c r="I10" t="s">
         <v>14</v>
@@ -5334,34 +5331,34 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B1" t="s">
         <v>260</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>261</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>262</v>
-      </c>
-      <c r="D1" t="s">
-        <v>263</v>
       </c>
       <c r="E1" t="s">
         <v>208</v>
       </c>
       <c r="F1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" t="s">
         <v>264</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" t="s">
         <v>266</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>267</v>
-      </c>
-      <c r="J1" t="s">
-        <v>268</v>
       </c>
       <c r="K1" t="s">
         <v>7</v>
@@ -5369,42 +5366,42 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B2" t="s">
         <v>269</v>
-      </c>
-      <c r="B2" t="s">
-        <v>270</v>
       </c>
       <c r="C2" t="s">
         <v>179</v>
       </c>
       <c r="D2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E2" t="s">
         <v>271</v>
-      </c>
-      <c r="E2" t="s">
-        <v>272</v>
       </c>
       <c r="F2" t="s">
         <v>211</v>
       </c>
       <c r="G2" t="s">
+        <v>272</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" t="s">
         <v>274</v>
-      </c>
-      <c r="I2" t="s">
-        <v>275</v>
       </c>
       <c r="J2" t="s">
         <v>51</v>
       </c>
       <c r="K2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B3" t="s">
         <v>218</v>
@@ -5413,33 +5410,33 @@
         <v>182</v>
       </c>
       <c r="D3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F3" t="s">
         <v>217</v>
       </c>
       <c r="G3" t="s">
+        <v>278</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" t="s">
         <v>280</v>
-      </c>
-      <c r="I3" t="s">
-        <v>281</v>
       </c>
       <c r="J3" t="s">
         <v>51</v>
       </c>
       <c r="K3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B4" t="s">
         <v>166</v>
@@ -5448,238 +5445,238 @@
         <v>185</v>
       </c>
       <c r="D4" t="s">
+        <v>283</v>
+      </c>
+      <c r="E4" t="s">
         <v>284</v>
-      </c>
-      <c r="E4" t="s">
-        <v>285</v>
       </c>
       <c r="F4" t="s">
         <v>185</v>
       </c>
       <c r="G4" t="s">
+        <v>285</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" t="s">
         <v>287</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>288</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>289</v>
-      </c>
-      <c r="K4" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C5" t="s">
         <v>188</v>
       </c>
       <c r="D5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G5" t="s">
+        <v>291</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" t="s">
         <v>293</v>
-      </c>
-      <c r="I5" t="s">
-        <v>294</v>
       </c>
       <c r="J5" t="s">
         <v>51</v>
       </c>
       <c r="K5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C6" t="s">
         <v>191</v>
       </c>
       <c r="D6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E6" t="s">
+        <v>296</v>
+      </c>
+      <c r="F6" t="s">
+        <v>232</v>
+      </c>
+      <c r="G6" t="s">
+        <v>285</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="F6" t="s">
-        <v>233</v>
-      </c>
-      <c r="G6" t="s">
-        <v>286</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" t="s">
         <v>298</v>
-      </c>
-      <c r="I6" t="s">
-        <v>299</v>
       </c>
       <c r="J6" t="s">
         <v>51</v>
       </c>
       <c r="K6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
+        <v>300</v>
+      </c>
+      <c r="B7" t="s">
         <v>301</v>
-      </c>
-      <c r="B7" t="s">
-        <v>302</v>
       </c>
       <c r="C7" t="s">
         <v>194</v>
       </c>
       <c r="D7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E7" t="s">
+        <v>302</v>
+      </c>
+      <c r="F7" t="s">
+        <v>237</v>
+      </c>
+      <c r="G7" t="s">
         <v>303</v>
       </c>
-      <c r="F7" t="s">
-        <v>238</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>305</v>
-      </c>
       <c r="I7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J7" t="s">
         <v>51</v>
       </c>
       <c r="K7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
+        <v>306</v>
+      </c>
+      <c r="B8" t="s">
         <v>307</v>
-      </c>
-      <c r="B8" t="s">
-        <v>308</v>
       </c>
       <c r="C8" t="s">
         <v>197</v>
       </c>
       <c r="D8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E8" t="s">
+        <v>308</v>
+      </c>
+      <c r="F8" t="s">
+        <v>242</v>
+      </c>
+      <c r="G8" t="s">
+        <v>303</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="F8" t="s">
-        <v>243</v>
-      </c>
-      <c r="G8" t="s">
-        <v>304</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" t="s">
         <v>310</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>311</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>312</v>
-      </c>
-      <c r="K8" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C9" t="s">
         <v>200</v>
       </c>
       <c r="D9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G9" t="s">
+        <v>314</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" t="s">
         <v>316</v>
-      </c>
-      <c r="I9" t="s">
-        <v>317</v>
       </c>
       <c r="J9" t="s">
         <v>51</v>
       </c>
       <c r="K9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
+        <v>318</v>
+      </c>
+      <c r="B10" t="s">
         <v>319</v>
-      </c>
-      <c r="B10" t="s">
-        <v>320</v>
       </c>
       <c r="C10" t="s">
         <v>203</v>
       </c>
       <c r="D10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E10" t="s">
+        <v>320</v>
+      </c>
+      <c r="F10" t="s">
         <v>321</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>322</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>324</v>
-      </c>
       <c r="I10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J10" t="s">
         <v>51</v>
       </c>
       <c r="K10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -5728,19 +5725,19 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F1" t="s">
         <v>326</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>327</v>
-      </c>
-      <c r="G1" t="s">
-        <v>328</v>
       </c>
       <c r="H1" t="s">
         <v>129</v>
       </c>
       <c r="I1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J1" t="s">
         <v>7</v>
@@ -5751,34 +5748,34 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B2" t="s">
         <v>330</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>331</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>332</v>
-      </c>
-      <c r="D2" t="s">
-        <v>333</v>
       </c>
       <c r="E2">
         <v>3</v>
       </c>
       <c r="F2" t="s">
+        <v>333</v>
+      </c>
+      <c r="G2" t="s">
         <v>334</v>
-      </c>
-      <c r="G2" t="s">
-        <v>335</v>
       </c>
       <c r="H2" t="s">
         <v>51</v>
       </c>
       <c r="I2" t="s">
+        <v>335</v>
+      </c>
+      <c r="J2" t="s">
         <v>336</v>
-      </c>
-      <c r="J2" t="s">
-        <v>337</v>
       </c>
       <c r="K2" t="s">
         <v>14</v>
@@ -5786,34 +5783,34 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
+        <v>337</v>
+      </c>
+      <c r="B3" t="s">
         <v>338</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>339</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>340</v>
-      </c>
-      <c r="D3" t="s">
-        <v>341</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H3" t="s">
         <v>51</v>
       </c>
       <c r="I3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K3" t="s">
         <v>14</v>
@@ -5821,34 +5818,34 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
+        <v>343</v>
+      </c>
+      <c r="B4" t="s">
         <v>344</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>345</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>346</v>
-      </c>
-      <c r="D4" t="s">
-        <v>347</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4" t="s">
+        <v>347</v>
+      </c>
+      <c r="G4" t="s">
         <v>348</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>349</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>350</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>351</v>
-      </c>
-      <c r="J4" t="s">
-        <v>352</v>
       </c>
       <c r="K4" t="s">
         <v>14</v>
@@ -5856,34 +5853,34 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
+        <v>352</v>
+      </c>
+      <c r="B5" t="s">
         <v>353</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>354</v>
       </c>
-      <c r="C5" t="s">
-        <v>355</v>
-      </c>
       <c r="D5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5" t="s">
+        <v>355</v>
+      </c>
+      <c r="G5" t="s">
+        <v>348</v>
+      </c>
+      <c r="H5" t="s">
+        <v>349</v>
+      </c>
+      <c r="I5" t="s">
+        <v>350</v>
+      </c>
+      <c r="J5" t="s">
         <v>356</v>
-      </c>
-      <c r="G5" t="s">
-        <v>349</v>
-      </c>
-      <c r="H5" t="s">
-        <v>350</v>
-      </c>
-      <c r="I5" t="s">
-        <v>351</v>
-      </c>
-      <c r="J5" t="s">
-        <v>357</v>
       </c>
       <c r="K5" t="s">
         <v>14</v>
@@ -5891,34 +5888,34 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
+        <v>357</v>
+      </c>
+      <c r="B6" t="s">
         <v>358</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>359</v>
       </c>
-      <c r="C6" t="s">
-        <v>360</v>
-      </c>
       <c r="D6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
       <c r="F6" t="s">
+        <v>360</v>
+      </c>
+      <c r="G6" t="s">
+        <v>348</v>
+      </c>
+      <c r="H6" t="s">
+        <v>349</v>
+      </c>
+      <c r="I6" t="s">
+        <v>350</v>
+      </c>
+      <c r="J6" t="s">
         <v>361</v>
-      </c>
-      <c r="G6" t="s">
-        <v>349</v>
-      </c>
-      <c r="H6" t="s">
-        <v>350</v>
-      </c>
-      <c r="I6" t="s">
-        <v>351</v>
-      </c>
-      <c r="J6" t="s">
-        <v>362</v>
       </c>
       <c r="K6" t="s">
         <v>14</v>
@@ -5926,34 +5923,34 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
+        <v>362</v>
+      </c>
+      <c r="B7" t="s">
         <v>363</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>364</v>
       </c>
-      <c r="C7" t="s">
-        <v>365</v>
-      </c>
       <c r="D7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H7" t="s">
         <v>51</v>
       </c>
       <c r="I7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K7" t="s">
         <v>14</v>
@@ -5961,34 +5958,34 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
+        <v>367</v>
+      </c>
+      <c r="B8" t="s">
         <v>368</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>369</v>
       </c>
-      <c r="C8" t="s">
-        <v>370</v>
-      </c>
       <c r="D8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H8" t="s">
         <v>51</v>
       </c>
       <c r="I8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K8" t="s">
         <v>14</v>
@@ -5996,34 +5993,34 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B9" t="s">
         <v>373</v>
       </c>
-      <c r="B9" t="s">
-        <v>374</v>
-      </c>
       <c r="C9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E9">
         <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H9" t="s">
         <v>51</v>
       </c>
       <c r="I9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K9" t="s">
         <v>14</v>
@@ -6031,34 +6028,34 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
+        <v>376</v>
+      </c>
+      <c r="B10" t="s">
         <v>377</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>378</v>
       </c>
-      <c r="C10" t="s">
-        <v>379</v>
-      </c>
       <c r="D10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E10">
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H10" t="s">
         <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="K10" t="s">
         <v>14</v>
@@ -6105,16 +6102,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>381</v>
+      </c>
+      <c r="E1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F1" t="s">
         <v>382</v>
       </c>
-      <c r="E1" t="s">
-        <v>326</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>383</v>
-      </c>
-      <c r="G1" t="s">
-        <v>384</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -6125,28 +6122,28 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B2" t="s">
         <v>385</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>386</v>
-      </c>
-      <c r="C2" t="s">
-        <v>387</v>
       </c>
       <c r="D2" t="s">
         <v>106</v>
       </c>
       <c r="E2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F2" t="s">
         <v>388</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>389</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>390</v>
-      </c>
-      <c r="H2" t="s">
-        <v>391</v>
       </c>
       <c r="I2" t="s">
         <v>14</v>
@@ -6154,28 +6151,28 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
+        <v>391</v>
+      </c>
+      <c r="B3" t="s">
         <v>392</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>393</v>
-      </c>
-      <c r="C3" t="s">
-        <v>394</v>
       </c>
       <c r="D3" t="s">
         <v>106</v>
       </c>
       <c r="E3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F3" t="s">
+        <v>394</v>
+      </c>
+      <c r="G3" t="s">
+        <v>389</v>
+      </c>
+      <c r="H3" t="s">
         <v>395</v>
-      </c>
-      <c r="G3" t="s">
-        <v>390</v>
-      </c>
-      <c r="H3" t="s">
-        <v>396</v>
       </c>
       <c r="I3" t="s">
         <v>14</v>
@@ -6183,28 +6180,28 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
+        <v>396</v>
+      </c>
+      <c r="B4" t="s">
         <v>397</v>
       </c>
-      <c r="B4" t="s">
-        <v>398</v>
-      </c>
       <c r="C4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D4" t="s">
         <v>106</v>
       </c>
       <c r="E4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I4" t="s">
         <v>14</v>
@@ -6212,28 +6209,28 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
+        <v>399</v>
+      </c>
+      <c r="B5" t="s">
         <v>400</v>
       </c>
-      <c r="B5" t="s">
-        <v>401</v>
-      </c>
       <c r="C5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D5" t="s">
         <v>106</v>
       </c>
       <c r="E5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I5" t="s">
         <v>14</v>
@@ -6241,28 +6238,28 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
+        <v>402</v>
+      </c>
+      <c r="B6" t="s">
         <v>403</v>
       </c>
-      <c r="B6" t="s">
-        <v>404</v>
-      </c>
       <c r="C6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D6" t="s">
         <v>106</v>
       </c>
       <c r="E6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I6" t="s">
         <v>14</v>
@@ -6270,28 +6267,28 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
+        <v>405</v>
+      </c>
+      <c r="B7" t="s">
         <v>406</v>
       </c>
-      <c r="B7" t="s">
-        <v>407</v>
-      </c>
       <c r="C7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D7" t="s">
         <v>106</v>
       </c>
       <c r="E7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H7" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="I7" t="s">
         <v>14</v>
@@ -6299,28 +6296,28 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
+        <v>408</v>
+      </c>
+      <c r="B8" t="s">
         <v>409</v>
       </c>
-      <c r="B8" t="s">
-        <v>410</v>
-      </c>
       <c r="C8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D8" t="s">
         <v>106</v>
       </c>
       <c r="E8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I8" t="s">
         <v>14</v>
@@ -6328,28 +6325,28 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
+        <v>411</v>
+      </c>
+      <c r="B9" t="s">
         <v>412</v>
       </c>
-      <c r="B9" t="s">
-        <v>413</v>
-      </c>
       <c r="C9" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D9" t="s">
         <v>106</v>
       </c>
       <c r="E9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F9" t="s">
+        <v>413</v>
+      </c>
+      <c r="G9" t="s">
+        <v>389</v>
+      </c>
+      <c r="H9" t="s">
         <v>414</v>
-      </c>
-      <c r="G9" t="s">
-        <v>390</v>
-      </c>
-      <c r="H9" t="s">
-        <v>415</v>
       </c>
       <c r="I9" t="s">
         <v>14</v>
@@ -6357,28 +6354,28 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D10" t="s">
         <v>106</v>
       </c>
       <c r="E10" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I10" t="s">
         <v>14</v>
@@ -6386,28 +6383,28 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B11" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D11" t="s">
         <v>106</v>
       </c>
       <c r="E11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F11" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G11" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H11" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I11" t="s">
         <v>14</v>
@@ -6415,28 +6412,28 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
+        <v>419</v>
+      </c>
+      <c r="B12" t="s">
         <v>420</v>
       </c>
-      <c r="B12" t="s">
-        <v>421</v>
-      </c>
       <c r="C12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D12" t="s">
         <v>106</v>
       </c>
       <c r="E12" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H12" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I12" t="s">
         <v>14</v>
@@ -6444,28 +6441,28 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
+        <v>422</v>
+      </c>
+      <c r="B13" t="s">
         <v>423</v>
       </c>
-      <c r="B13" t="s">
-        <v>424</v>
-      </c>
       <c r="C13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D13" t="s">
         <v>106</v>
       </c>
       <c r="E13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H13" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I13" t="s">
         <v>14</v>
@@ -6473,28 +6470,28 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
+        <v>425</v>
+      </c>
+      <c r="B14" t="s">
         <v>426</v>
       </c>
-      <c r="B14" t="s">
-        <v>427</v>
-      </c>
       <c r="C14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D14" t="s">
         <v>106</v>
       </c>
       <c r="E14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H14" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I14" t="s">
         <v>14</v>

</xml_diff>